<commit_message>
Adding update to gnatt chart progress
</commit_message>
<xml_diff>
--- a/Gnatt Chart/Agile Gantt Chart.xlsx
+++ b/Gnatt Chart/Agile Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308E0E4B-8F73-490E-9677-A59B36B0C395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF4539-B8E4-44E3-9B1A-0DBBBA773CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dark" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -879,6 +879,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -891,16 +894,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1483,7 +1483,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>31750</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
@@ -1491,7 +1491,7 @@
           <xdr:col>64</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1826,51 +1826,51 @@
   </sheetPr>
   <dimension ref="A1:BP63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A53" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="9" customWidth="1"/>
-    <col min="9" max="21" width="3.5703125" style="9" customWidth="1"/>
-    <col min="22" max="22" width="3.42578125" style="9" customWidth="1"/>
-    <col min="23" max="64" width="3.5703125" style="9" customWidth="1"/>
-    <col min="65" max="65" width="2.7109375" style="9" customWidth="1"/>
-    <col min="66" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="4.7265625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" style="9" customWidth="1"/>
+    <col min="9" max="21" width="3.54296875" style="9" customWidth="1"/>
+    <col min="22" max="22" width="3.453125" style="9" customWidth="1"/>
+    <col min="23" max="64" width="3.54296875" style="9" customWidth="1"/>
+    <col min="65" max="65" width="2.7265625" style="9" customWidth="1"/>
+    <col min="66" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
@@ -1917,7 +1917,7 @@
       <c r="BL2" s="19"/>
       <c r="BM2" s="19"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="43"/>
       <c r="C3" s="44"/>
@@ -1984,7 +1984,7 @@
       <c r="BL3" s="32"/>
       <c r="BM3" s="30"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="57" t="s">
         <v>17</v>
@@ -1997,33 +1997,33 @@
         <v>11</v>
       </c>
       <c r="H4" s="27"/>
-      <c r="I4" s="79" t="s">
+      <c r="I4" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
       <c r="M4" s="30"/>
-      <c r="N4" s="77" t="s">
+      <c r="N4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="78" t="s">
+      <c r="S4" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
       <c r="W4" s="30"/>
-      <c r="X4" s="80" t="s">
+      <c r="X4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="80"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
       <c r="AD4" s="30"/>
@@ -2063,7 +2063,7 @@
       <c r="BL4" s="30"/>
       <c r="BM4" s="30"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="58" t="s">
         <v>19</v>
@@ -2132,7 +2132,7 @@
       <c r="BL5" s="32"/>
       <c r="BM5" s="30"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="7"/>
       <c r="B6" s="51" t="s">
         <v>10</v>
@@ -2227,7 +2227,7 @@
       <c r="BL6" s="63"/>
       <c r="BM6" s="30"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="51" t="s">
         <v>5</v>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="BM7" s="30"/>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -2533,7 +2533,7 @@
       <c r="BL8" s="40"/>
       <c r="BM8" s="30"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="70" t="s">
         <v>13</v>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="BM9" s="30"/>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="15"/>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
@@ -2846,7 +2846,7 @@
       <c r="BL10" s="37"/>
       <c r="BM10" s="30"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="24" t="s">
         <v>22</v>
@@ -3094,7 +3094,7 @@
       <c r="BM11" s="26"/>
       <c r="BP11" s="42"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="24" t="s">
         <v>23</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="BM12" s="26"/>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="24" t="s">
         <v>57</v>
@@ -3420,7 +3420,7 @@
       <c r="BL13" s="25"/>
       <c r="BM13" s="26"/>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="24" t="s">
         <v>58</v>
@@ -3499,7 +3499,7 @@
       <c r="BL14" s="25"/>
       <c r="BM14" s="26"/>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="24" t="s">
         <v>29</v>
@@ -3578,7 +3578,7 @@
       <c r="BL15" s="25"/>
       <c r="BM15" s="26"/>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="24" t="s">
         <v>24</v>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="BM16" s="26"/>
     </row>
-    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="BM17" s="26"/>
     </row>
-    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="24" t="s">
         <v>25</v>
@@ -4319,7 +4319,7 @@
       </c>
       <c r="BM18" s="26"/>
     </row>
-    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="24" t="s">
         <v>27</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="BM19" s="26"/>
     </row>
-    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="24" t="s">
         <v>41</v>
@@ -4643,7 +4643,7 @@
       <c r="BL20" s="25"/>
       <c r="BM20" s="26"/>
     </row>
-    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="24" t="s">
         <v>67</v>
@@ -4722,7 +4722,7 @@
       <c r="BL21" s="25"/>
       <c r="BM21" s="26"/>
     </row>
-    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="24" t="s">
         <v>26</v>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="BM22" s="26"/>
     </row>
-    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="24" t="s">
         <v>30</v>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="BM23" s="26"/>
     </row>
-    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="24" t="s">
         <v>42</v>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="BM24" s="26"/>
     </row>
-    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="24" t="s">
         <v>68</v>
@@ -5542,7 +5542,7 @@
       <c r="BL25" s="25"/>
       <c r="BM25" s="26"/>
     </row>
-    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>31</v>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="BM26" s="26"/>
     </row>
-    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="24" t="s">
         <v>43</v>
@@ -6036,7 +6036,7 @@
       </c>
       <c r="BM27" s="26"/>
     </row>
-    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="24" t="s">
         <v>33</v>
@@ -6283,7 +6283,7 @@
       </c>
       <c r="BM28" s="26"/>
     </row>
-    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="24" t="s">
         <v>44</v>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="BM29" s="26"/>
     </row>
-    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="24" t="s">
         <v>32</v>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="BM30" s="26"/>
     </row>
-    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="24" t="s">
         <v>45</v>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="BM31" s="26"/>
     </row>
-    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="24" t="s">
         <v>34</v>
@@ -7272,7 +7272,7 @@
       </c>
       <c r="BM32" s="26"/>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="24" t="s">
         <v>47</v>
@@ -7351,7 +7351,7 @@
       <c r="BL33" s="25"/>
       <c r="BM33" s="26"/>
     </row>
-    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="24" t="s">
         <v>48</v>
@@ -7430,7 +7430,7 @@
       <c r="BL34" s="25"/>
       <c r="BM34" s="26"/>
     </row>
-    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="24" t="s">
         <v>46</v>
@@ -7678,7 +7678,7 @@
       </c>
       <c r="BM35" s="26"/>
     </row>
-    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="24" t="s">
         <v>35</v>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="BM36" s="26"/>
     </row>
-    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="24" t="s">
         <v>36</v>
@@ -8172,7 +8172,7 @@
       </c>
       <c r="BM37" s="26"/>
     </row>
-    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="24" t="s">
         <v>37</v>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="BM38" s="26"/>
     </row>
-    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="24" t="s">
         <v>38</v>
@@ -8666,19 +8666,19 @@
       </c>
       <c r="BM39" s="26"/>
     </row>
-    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E40" s="21">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F40" s="22">
         <v>44511</v>
@@ -8913,24 +8913,26 @@
       </c>
       <c r="BM40" s="26"/>
     </row>
-    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="22">
         <v>44511</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="23">
+        <v>2</v>
+      </c>
       <c r="H41" s="18"/>
       <c r="I41" s="49" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -9158,7 +9160,7 @@
       </c>
       <c r="BM41" s="26"/>
     </row>
-    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="24" t="s">
         <v>49</v>
@@ -9399,7 +9401,7 @@
       </c>
       <c r="BM42" s="26"/>
     </row>
-    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="24" t="s">
         <v>69</v>
@@ -9468,7 +9470,7 @@
       <c r="BL43" s="25"/>
       <c r="BM43" s="26"/>
     </row>
-    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="24" t="s">
         <v>50</v>
@@ -9537,7 +9539,7 @@
       <c r="BL44" s="25"/>
       <c r="BM44" s="26"/>
     </row>
-    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="24" t="s">
         <v>51</v>
@@ -9608,7 +9610,7 @@
       <c r="BL45" s="25"/>
       <c r="BM45" s="26"/>
     </row>
-    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="24" t="s">
         <v>52</v>
@@ -9679,15 +9681,23 @@
       <c r="BL46" s="25"/>
       <c r="BM46" s="26"/>
     </row>
-    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="22"/>
+      <c r="C47" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="F47" s="22">
+        <v>44513</v>
+      </c>
       <c r="G47" s="23"/>
       <c r="H47" s="18"/>
       <c r="I47" s="49"/>
@@ -9748,15 +9758,23 @@
       <c r="BL47" s="25"/>
       <c r="BM47" s="26"/>
     </row>
-    <row r="48" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="22"/>
+      <c r="C48" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="F48" s="22">
+        <v>44513</v>
+      </c>
       <c r="G48" s="23"/>
       <c r="H48" s="18"/>
       <c r="I48" s="49"/>
@@ -9817,7 +9835,7 @@
       <c r="BL48" s="25"/>
       <c r="BM48" s="26"/>
     </row>
-    <row r="49" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" s="24" t="s">
         <v>70</v>
@@ -9888,7 +9906,7 @@
       <c r="BL49" s="25"/>
       <c r="BM49" s="26"/>
     </row>
-    <row r="50" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="24" t="s">
         <v>53</v>
@@ -10127,7 +10145,7 @@
       </c>
       <c r="BM50" s="65"/>
     </row>
-    <row r="51" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" s="24" t="s">
         <v>56</v>
@@ -10196,7 +10214,7 @@
       <c r="BL51" s="64"/>
       <c r="BM51" s="47"/>
     </row>
-    <row r="52" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="24" t="s">
         <v>59</v>
@@ -10265,7 +10283,7 @@
       <c r="BL52" s="64"/>
       <c r="BM52" s="47"/>
     </row>
-    <row r="53" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6"/>
       <c r="B53" s="24" t="s">
         <v>60</v>
@@ -10334,7 +10352,7 @@
       <c r="BL53" s="64"/>
       <c r="BM53" s="47"/>
     </row>
-    <row r="54" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
       <c r="B54" s="24" t="s">
         <v>61</v>
@@ -10403,7 +10421,7 @@
       <c r="BL54" s="64"/>
       <c r="BM54" s="47"/>
     </row>
-    <row r="55" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="24" t="s">
         <v>62</v>
@@ -10472,7 +10490,7 @@
       <c r="BL55" s="64"/>
       <c r="BM55" s="47"/>
     </row>
-    <row r="56" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="24" t="s">
         <v>65</v>
@@ -10543,7 +10561,7 @@
       <c r="BL56" s="64"/>
       <c r="BM56" s="47"/>
     </row>
-    <row r="57" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="24" t="s">
         <v>63</v>
@@ -10612,7 +10630,7 @@
       <c r="BL57" s="64"/>
       <c r="BM57" s="47"/>
     </row>
-    <row r="58" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="24" t="s">
         <v>66</v>
@@ -10683,7 +10701,7 @@
       <c r="BL58" s="64"/>
       <c r="BM58" s="47"/>
     </row>
-    <row r="59" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" s="24" t="s">
         <v>64</v>
@@ -10752,7 +10770,7 @@
       <c r="BL59" s="64"/>
       <c r="BM59" s="47"/>
     </row>
-    <row r="60" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="72"/>
       <c r="C60" s="20"/>
@@ -10819,7 +10837,7 @@
       <c r="BL60" s="64"/>
       <c r="BM60" s="47"/>
     </row>
-    <row r="61" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
       <c r="B61" s="69" t="s">
         <v>12</v>
@@ -10888,12 +10906,12 @@
       <c r="BL61" s="64"/>
       <c r="BM61" s="47"/>
     </row>
-    <row r="62" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D62" s="4"/>
       <c r="G62" s="8"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D63" s="5"/>
     </row>
   </sheetData>
@@ -11013,7 +11031,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>31750</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>57150</xdr:rowOff>
                   </from>
@@ -11021,7 +11039,7 @@
                     <xdr:col>64</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11097,25 +11115,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11391,6 +11390,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11401,18 +11419,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11433,6 +11439,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adding status reports and updated gantt chart:
</commit_message>
<xml_diff>
--- a/Gnatt Chart/Agile Gantt Chart.xlsx
+++ b/Gnatt Chart/Agile Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF4539-B8E4-44E3-9B1A-0DBBBA773CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8E5548-F308-423E-8452-C623EFD276E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dark" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Create mock image of recommendation UI</t>
+  </si>
+  <si>
+    <t>Group Status Report 9</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -878,6 +881,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1483,7 +1489,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>31750</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
@@ -1491,7 +1497,7 @@
           <xdr:col>64</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1532,8 +1538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G61" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="B9:G61" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G62" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B9:G62" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1824,53 +1830,53 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BP63"/>
+  <dimension ref="A1:BP64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A53" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="2.7265625" style="9" customWidth="1"/>
-    <col min="9" max="21" width="3.54296875" style="9" customWidth="1"/>
-    <col min="22" max="22" width="3.453125" style="9" customWidth="1"/>
-    <col min="23" max="64" width="3.54296875" style="9" customWidth="1"/>
-    <col min="65" max="65" width="2.7265625" style="9" customWidth="1"/>
-    <col min="66" max="16384" width="8.81640625" style="9"/>
+    <col min="1" max="1" width="4.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="9" customWidth="1"/>
+    <col min="9" max="21" width="3.5703125" style="9" customWidth="1"/>
+    <col min="22" max="22" width="3.42578125" style="9" customWidth="1"/>
+    <col min="23" max="64" width="3.5703125" style="9" customWidth="1"/>
+    <col min="65" max="65" width="2.7109375" style="9" customWidth="1"/>
+    <col min="66" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
@@ -1917,7 +1923,7 @@
       <c r="BL2" s="19"/>
       <c r="BM2" s="19"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="43"/>
       <c r="C3" s="44"/>
@@ -1984,7 +1990,7 @@
       <c r="BL3" s="32"/>
       <c r="BM3" s="30"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="57" t="s">
         <v>17</v>
@@ -1997,33 +2003,33 @@
         <v>11</v>
       </c>
       <c r="H4" s="27"/>
-      <c r="I4" s="78" t="s">
+      <c r="I4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
       <c r="M4" s="30"/>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
       <c r="W4" s="30"/>
-      <c r="X4" s="73" t="s">
+      <c r="X4" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
       <c r="AD4" s="30"/>
@@ -2063,7 +2069,7 @@
       <c r="BL4" s="30"/>
       <c r="BM4" s="30"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="58" t="s">
         <v>19</v>
@@ -2132,7 +2138,7 @@
       <c r="BL5" s="32"/>
       <c r="BM5" s="30"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="51" t="s">
         <v>10</v>
@@ -2227,7 +2233,7 @@
       <c r="BL6" s="63"/>
       <c r="BM6" s="30"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="51" t="s">
         <v>5</v>
@@ -2466,7 +2472,7 @@
       </c>
       <c r="BM7" s="30"/>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -2533,7 +2539,7 @@
       <c r="BL8" s="40"/>
       <c r="BM8" s="30"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="70" t="s">
         <v>13</v>
@@ -2780,7 +2786,7 @@
       </c>
       <c r="BM9" s="30"/>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
@@ -2846,7 +2852,7 @@
       <c r="BL10" s="37"/>
       <c r="BM10" s="30"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="24" t="s">
         <v>22</v>
@@ -3094,7 +3100,7 @@
       <c r="BM11" s="26"/>
       <c r="BP11" s="42"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="24" t="s">
         <v>23</v>
@@ -3341,7 +3347,7 @@
       </c>
       <c r="BM12" s="26"/>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="24" t="s">
         <v>57</v>
@@ -3420,7 +3426,7 @@
       <c r="BL13" s="25"/>
       <c r="BM13" s="26"/>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="24" t="s">
         <v>58</v>
@@ -3499,7 +3505,7 @@
       <c r="BL14" s="25"/>
       <c r="BM14" s="26"/>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="24" t="s">
         <v>29</v>
@@ -3578,7 +3584,7 @@
       <c r="BL15" s="25"/>
       <c r="BM15" s="26"/>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="24" t="s">
         <v>24</v>
@@ -3825,7 +3831,7 @@
       </c>
       <c r="BM16" s="26"/>
     </row>
-    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -4072,7 +4078,7 @@
       </c>
       <c r="BM17" s="26"/>
     </row>
-    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="24" t="s">
         <v>25</v>
@@ -4319,7 +4325,7 @@
       </c>
       <c r="BM18" s="26"/>
     </row>
-    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="24" t="s">
         <v>27</v>
@@ -4566,7 +4572,7 @@
       </c>
       <c r="BM19" s="26"/>
     </row>
-    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="24" t="s">
         <v>41</v>
@@ -4578,7 +4584,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="21">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F20" s="22">
         <v>44470</v>
@@ -4643,7 +4649,7 @@
       <c r="BL20" s="25"/>
       <c r="BM20" s="26"/>
     </row>
-    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="24" t="s">
         <v>67</v>
@@ -4722,7 +4728,7 @@
       <c r="BL21" s="25"/>
       <c r="BM21" s="26"/>
     </row>
-    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="24" t="s">
         <v>26</v>
@@ -4969,7 +4975,7 @@
       </c>
       <c r="BM22" s="26"/>
     </row>
-    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="24" t="s">
         <v>30</v>
@@ -5216,7 +5222,7 @@
       </c>
       <c r="BM23" s="26"/>
     </row>
-    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="24" t="s">
         <v>42</v>
@@ -5463,7 +5469,7 @@
       </c>
       <c r="BM24" s="26"/>
     </row>
-    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="24" t="s">
         <v>68</v>
@@ -5542,7 +5548,7 @@
       <c r="BL25" s="25"/>
       <c r="BM25" s="26"/>
     </row>
-    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>31</v>
@@ -5789,7 +5795,7 @@
       </c>
       <c r="BM26" s="26"/>
     </row>
-    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="24" t="s">
         <v>43</v>
@@ -6036,7 +6042,7 @@
       </c>
       <c r="BM27" s="26"/>
     </row>
-    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="24" t="s">
         <v>33</v>
@@ -6283,7 +6289,7 @@
       </c>
       <c r="BM28" s="26"/>
     </row>
-    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="24" t="s">
         <v>44</v>
@@ -6530,7 +6536,7 @@
       </c>
       <c r="BM29" s="26"/>
     </row>
-    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="24" t="s">
         <v>32</v>
@@ -6777,7 +6783,7 @@
       </c>
       <c r="BM30" s="26"/>
     </row>
-    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="24" t="s">
         <v>45</v>
@@ -7025,7 +7031,7 @@
       </c>
       <c r="BM31" s="26"/>
     </row>
-    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="24" t="s">
         <v>34</v>
@@ -7171,7 +7177,7 @@
         <v/>
       </c>
       <c r="AN32" s="25" t="str">
-        <f t="shared" ref="AN32:BC50" ca="1" si="9">IF(AND($C32="Goal",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),1,""))</f>
+        <f t="shared" ref="AN32:BC51" ca="1" si="9">IF(AND($C32="Goal",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AO32" s="25" t="str">
@@ -7235,7 +7241,7 @@
         <v/>
       </c>
       <c r="BD32" s="25" t="str">
-        <f t="shared" ref="BD32:BL50" ca="1" si="10">IF(AND($C32="Goal",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),1,""))</f>
+        <f t="shared" ref="BD32:BL51" ca="1" si="10">IF(AND($C32="Goal",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BE32" s="25" t="str">
@@ -7272,7 +7278,7 @@
       </c>
       <c r="BM32" s="26"/>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="24" t="s">
         <v>47</v>
@@ -7351,7 +7357,7 @@
       <c r="BL33" s="25"/>
       <c r="BM33" s="26"/>
     </row>
-    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="24" t="s">
         <v>48</v>
@@ -7430,7 +7436,7 @@
       <c r="BL34" s="25"/>
       <c r="BM34" s="26"/>
     </row>
-    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="24" t="s">
         <v>46</v>
@@ -7678,7 +7684,7 @@
       </c>
       <c r="BM35" s="26"/>
     </row>
-    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="24" t="s">
         <v>35</v>
@@ -7764,7 +7770,7 @@
         <v/>
       </c>
       <c r="Y36" s="25" t="str">
-        <f t="shared" ref="Y36:AM50" ca="1" si="13">IF(AND($C36="Goal",Y$7&gt;=$F36,Y$7&lt;=$F36+$G36-1),2,IF(AND($C36="Milestone",Y$7&gt;=$F36,Y$7&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ref="Y36:AM51" ca="1" si="13">IF(AND($C36="Goal",Y$7&gt;=$F36,Y$7&lt;=$F36+$G36-1),2,IF(AND($C36="Milestone",Y$7&gt;=$F36,Y$7&lt;=$F36+$G36-1),1,""))</f>
         <v/>
       </c>
       <c r="Z36" s="25" t="str">
@@ -7925,7 +7931,7 @@
       </c>
       <c r="BM36" s="26"/>
     </row>
-    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="24" t="s">
         <v>36</v>
@@ -8172,7 +8178,7 @@
       </c>
       <c r="BM37" s="26"/>
     </row>
-    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="24" t="s">
         <v>37</v>
@@ -8194,7 +8200,7 @@
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="49" t="str">
-        <f t="shared" ref="I38:X50" ca="1" si="15">IF(AND($C38="Goal",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),1,""))</f>
+        <f t="shared" ref="I38:X51" ca="1" si="15">IF(AND($C38="Goal",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="J38" s="25" t="str">
@@ -8419,7 +8425,7 @@
       </c>
       <c r="BM38" s="26"/>
     </row>
-    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="24" t="s">
         <v>38</v>
@@ -8666,7 +8672,7 @@
       </c>
       <c r="BM39" s="26"/>
     </row>
-    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="24" t="s">
         <v>39</v>
@@ -8913,7 +8919,7 @@
       </c>
       <c r="BM40" s="26"/>
     </row>
-    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="24" t="s">
         <v>40</v>
@@ -9160,7 +9166,7 @@
       </c>
       <c r="BM41" s="26"/>
     </row>
-    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="24" t="s">
         <v>49</v>
@@ -9171,9 +9177,15 @@
       <c r="D42" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
+      <c r="E42" s="21">
+        <v>1</v>
+      </c>
+      <c r="F42" s="22">
+        <v>44514</v>
+      </c>
+      <c r="G42" s="23">
+        <v>3</v>
+      </c>
       <c r="H42" s="18"/>
       <c r="I42" s="49" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -9401,16 +9413,26 @@
       </c>
       <c r="BM42" s="26"/>
     </row>
-    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="21">
+        <v>1</v>
+      </c>
+      <c r="F43" s="22">
+        <v>44515</v>
+      </c>
+      <c r="G43" s="23">
+        <v>1</v>
+      </c>
       <c r="H43" s="18"/>
       <c r="I43" s="49"/>
       <c r="J43" s="25"/>
@@ -9470,10 +9492,10 @@
       <c r="BL43" s="25"/>
       <c r="BM43" s="26"/>
     </row>
-    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="24" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -9539,18 +9561,26 @@
       <c r="BL44" s="25"/>
       <c r="BM44" s="26"/>
     </row>
-    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="20"/>
+        <v>50</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="D45" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="E45" s="21">
+        <v>1</v>
+      </c>
+      <c r="F45" s="22">
+        <v>44516</v>
+      </c>
+      <c r="G45" s="23">
+        <v>1</v>
+      </c>
       <c r="H45" s="18"/>
       <c r="I45" s="49"/>
       <c r="J45" s="25"/>
@@ -9610,14 +9640,14 @@
       <c r="BL45" s="25"/>
       <c r="BM45" s="26"/>
     </row>
-    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E46" s="21"/>
       <c r="F46" s="22"/>
@@ -9681,23 +9711,17 @@
       <c r="BL46" s="25"/>
       <c r="BM46" s="26"/>
     </row>
-    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>6</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C47" s="20"/>
       <c r="D47" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="F47" s="22">
-        <v>44513</v>
-      </c>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22"/>
       <c r="G47" s="23"/>
       <c r="H47" s="18"/>
       <c r="I47" s="49"/>
@@ -9758,10 +9782,10 @@
       <c r="BL47" s="25"/>
       <c r="BM47" s="26"/>
     </row>
-    <row r="48" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>6</v>
@@ -9835,17 +9859,23 @@
       <c r="BL48" s="25"/>
       <c r="BM48" s="26"/>
     </row>
-    <row r="49" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>6</v>
+      </c>
       <c r="D49" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="21"/>
-      <c r="F49" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="E49" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="F49" s="22">
+        <v>44513</v>
+      </c>
       <c r="G49" s="23"/>
       <c r="H49" s="18"/>
       <c r="I49" s="49"/>
@@ -9906,318 +9936,326 @@
       <c r="BL49" s="25"/>
       <c r="BM49" s="26"/>
     </row>
-    <row r="50" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="24" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C50" s="20"/>
       <c r="D50" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E50" s="21"/>
       <c r="F50" s="22"/>
       <c r="G50" s="23"/>
       <c r="H50" s="18"/>
-      <c r="I50" s="49" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="J50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="K50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="L50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="M50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="N50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="O50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="P50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="Q50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="R50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="S50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="T50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="U50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="V50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="W50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="X50" s="25" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="Y50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="Z50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AA50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AB50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AC50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AD50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AE50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AF50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AG50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AH50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AI50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AJ50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AK50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AL50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AM50" s="25" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AN50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AP50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AQ50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AR50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AS50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AT50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AU50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AV50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AW50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AX50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AY50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AZ50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BA50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BB50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BC50" s="25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BD50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BE50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BF50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BG50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BH50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BI50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BJ50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BK50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BL50" s="25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BM50" s="65"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="25"/>
+      <c r="T50" s="25"/>
+      <c r="U50" s="25"/>
+      <c r="V50" s="25"/>
+      <c r="W50" s="25"/>
+      <c r="X50" s="25"/>
+      <c r="Y50" s="25"/>
+      <c r="Z50" s="25"/>
+      <c r="AA50" s="25"/>
+      <c r="AB50" s="25"/>
+      <c r="AC50" s="25"/>
+      <c r="AD50" s="25"/>
+      <c r="AE50" s="25"/>
+      <c r="AF50" s="25"/>
+      <c r="AG50" s="25"/>
+      <c r="AH50" s="25"/>
+      <c r="AI50" s="25"/>
+      <c r="AJ50" s="25"/>
+      <c r="AK50" s="25"/>
+      <c r="AL50" s="25"/>
+      <c r="AM50" s="25"/>
+      <c r="AN50" s="25"/>
+      <c r="AO50" s="25"/>
+      <c r="AP50" s="25"/>
+      <c r="AQ50" s="25"/>
+      <c r="AR50" s="25"/>
+      <c r="AS50" s="25"/>
+      <c r="AT50" s="25"/>
+      <c r="AU50" s="25"/>
+      <c r="AV50" s="25"/>
+      <c r="AW50" s="25"/>
+      <c r="AX50" s="25"/>
+      <c r="AY50" s="25"/>
+      <c r="AZ50" s="25"/>
+      <c r="BA50" s="25"/>
+      <c r="BB50" s="25"/>
+      <c r="BC50" s="25"/>
+      <c r="BD50" s="25"/>
+      <c r="BE50" s="25"/>
+      <c r="BF50" s="25"/>
+      <c r="BG50" s="25"/>
+      <c r="BH50" s="25"/>
+      <c r="BI50" s="25"/>
+      <c r="BJ50" s="25"/>
+      <c r="BK50" s="25"/>
+      <c r="BL50" s="25"/>
+      <c r="BM50" s="26"/>
     </row>
-    <row r="51" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="22"/>
+        <v>53</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="22">
+        <v>44519</v>
+      </c>
       <c r="G51" s="23"/>
       <c r="H51" s="18"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
-      <c r="M51" s="64"/>
-      <c r="N51" s="64"/>
-      <c r="O51" s="64"/>
-      <c r="P51" s="64"/>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="64"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="64"/>
-      <c r="U51" s="64"/>
-      <c r="V51" s="64"/>
-      <c r="W51" s="64"/>
-      <c r="X51" s="64"/>
-      <c r="Y51" s="64"/>
-      <c r="Z51" s="64"/>
-      <c r="AA51" s="64"/>
-      <c r="AB51" s="64"/>
-      <c r="AC51" s="64"/>
-      <c r="AD51" s="64"/>
-      <c r="AE51" s="64"/>
-      <c r="AF51" s="64"/>
-      <c r="AG51" s="64"/>
-      <c r="AH51" s="64"/>
-      <c r="AI51" s="64"/>
-      <c r="AJ51" s="64"/>
-      <c r="AK51" s="64"/>
-      <c r="AL51" s="64"/>
-      <c r="AM51" s="64"/>
-      <c r="AN51" s="64"/>
-      <c r="AO51" s="64"/>
-      <c r="AP51" s="64"/>
-      <c r="AQ51" s="64"/>
-      <c r="AR51" s="64"/>
-      <c r="AS51" s="64"/>
-      <c r="AT51" s="64"/>
-      <c r="AU51" s="64"/>
-      <c r="AV51" s="64"/>
-      <c r="AW51" s="64"/>
-      <c r="AX51" s="64"/>
-      <c r="AY51" s="64"/>
-      <c r="AZ51" s="64"/>
-      <c r="BA51" s="64"/>
-      <c r="BB51" s="64"/>
-      <c r="BC51" s="64"/>
-      <c r="BD51" s="64"/>
-      <c r="BE51" s="64"/>
-      <c r="BF51" s="64"/>
-      <c r="BG51" s="64"/>
-      <c r="BH51" s="64"/>
-      <c r="BI51" s="64"/>
-      <c r="BJ51" s="64"/>
-      <c r="BK51" s="64"/>
-      <c r="BL51" s="64"/>
-      <c r="BM51" s="47"/>
+      <c r="I51" s="49" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="J51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="K51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="L51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="M51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="N51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="O51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="P51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="Q51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="R51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="S51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="T51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="U51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="V51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="W51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="X51" s="25" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="Y51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="Z51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AA51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AB51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AC51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AD51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AE51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AF51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AG51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AH51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AI51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AJ51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AK51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AL51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AM51" s="25" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AN51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AO51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AP51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AQ51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AR51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AS51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AV51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AW51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AX51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AY51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AZ51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BA51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BB51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BC51" s="25" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BD51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BE51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BF51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BG51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BH51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BI51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BJ51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BK51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BL51" s="25" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BM51" s="65"/>
     </row>
-    <row r="52" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
@@ -10283,10 +10321,10 @@
       <c r="BL52" s="64"/>
       <c r="BM52" s="47"/>
     </row>
-    <row r="53" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -10352,16 +10390,24 @@
       <c r="BL53" s="64"/>
       <c r="BM53" s="47"/>
     </row>
-    <row r="54" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="23"/>
+      <c r="D54" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="21">
+        <v>1</v>
+      </c>
+      <c r="F54" s="22">
+        <v>44516</v>
+      </c>
+      <c r="G54" s="23">
+        <v>1</v>
+      </c>
       <c r="H54" s="18"/>
       <c r="I54" s="64"/>
       <c r="J54" s="64"/>
@@ -10421,10 +10467,10 @@
       <c r="BL54" s="64"/>
       <c r="BM54" s="47"/>
     </row>
-    <row r="55" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="20"/>
       <c r="D55" s="20"/>
@@ -10490,15 +10536,13 @@
       <c r="BL55" s="64"/>
       <c r="BM55" s="47"/>
     </row>
-    <row r="56" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C56" s="20"/>
-      <c r="D56" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="D56" s="20"/>
       <c r="E56" s="21"/>
       <c r="F56" s="22"/>
       <c r="G56" s="23"/>
@@ -10561,13 +10605,15 @@
       <c r="BL56" s="64"/>
       <c r="BM56" s="47"/>
     </row>
-    <row r="57" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
+      <c r="D57" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E57" s="21"/>
       <c r="F57" s="22"/>
       <c r="G57" s="23"/>
@@ -10630,15 +10676,13 @@
       <c r="BL57" s="64"/>
       <c r="BM57" s="47"/>
     </row>
-    <row r="58" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58" s="20"/>
-      <c r="D58" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="D58" s="20"/>
       <c r="E58" s="21"/>
       <c r="F58" s="22"/>
       <c r="G58" s="23"/>
@@ -10701,13 +10745,15 @@
       <c r="BL58" s="64"/>
       <c r="BM58" s="47"/>
     </row>
-    <row r="59" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
+      <c r="D59" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E59" s="21"/>
       <c r="F59" s="22"/>
       <c r="G59" s="23"/>
@@ -10770,9 +10816,11 @@
       <c r="BL59" s="64"/>
       <c r="BM59" s="47"/>
     </row>
-    <row r="60" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="72"/>
+      <c r="B60" s="24" t="s">
+        <v>64</v>
+      </c>
       <c r="C60" s="20"/>
       <c r="D60" s="20"/>
       <c r="E60" s="21"/>
@@ -10837,16 +10885,14 @@
       <c r="BL60" s="64"/>
       <c r="BM60" s="47"/>
     </row>
-    <row r="61" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="7"/>
-      <c r="B61" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="61"/>
+    <row r="61" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="23"/>
       <c r="H61" s="18"/>
       <c r="I61" s="64"/>
       <c r="J61" s="64"/>
@@ -10906,13 +10952,82 @@
       <c r="BL61" s="64"/>
       <c r="BM61" s="47"/>
     </row>
-    <row r="62" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="4"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="3"/>
+    <row r="62" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="64"/>
+      <c r="J62" s="64"/>
+      <c r="K62" s="64"/>
+      <c r="L62" s="64"/>
+      <c r="M62" s="64"/>
+      <c r="N62" s="64"/>
+      <c r="O62" s="64"/>
+      <c r="P62" s="64"/>
+      <c r="Q62" s="64"/>
+      <c r="R62" s="64"/>
+      <c r="S62" s="64"/>
+      <c r="T62" s="64"/>
+      <c r="U62" s="64"/>
+      <c r="V62" s="64"/>
+      <c r="W62" s="64"/>
+      <c r="X62" s="64"/>
+      <c r="Y62" s="64"/>
+      <c r="Z62" s="64"/>
+      <c r="AA62" s="64"/>
+      <c r="AB62" s="64"/>
+      <c r="AC62" s="64"/>
+      <c r="AD62" s="64"/>
+      <c r="AE62" s="64"/>
+      <c r="AF62" s="64"/>
+      <c r="AG62" s="64"/>
+      <c r="AH62" s="64"/>
+      <c r="AI62" s="64"/>
+      <c r="AJ62" s="64"/>
+      <c r="AK62" s="64"/>
+      <c r="AL62" s="64"/>
+      <c r="AM62" s="64"/>
+      <c r="AN62" s="64"/>
+      <c r="AO62" s="64"/>
+      <c r="AP62" s="64"/>
+      <c r="AQ62" s="64"/>
+      <c r="AR62" s="64"/>
+      <c r="AS62" s="64"/>
+      <c r="AT62" s="64"/>
+      <c r="AU62" s="64"/>
+      <c r="AV62" s="64"/>
+      <c r="AW62" s="64"/>
+      <c r="AX62" s="64"/>
+      <c r="AY62" s="64"/>
+      <c r="AZ62" s="64"/>
+      <c r="BA62" s="64"/>
+      <c r="BB62" s="64"/>
+      <c r="BC62" s="64"/>
+      <c r="BD62" s="64"/>
+      <c r="BE62" s="64"/>
+      <c r="BF62" s="64"/>
+      <c r="BG62" s="64"/>
+      <c r="BH62" s="64"/>
+      <c r="BI62" s="64"/>
+      <c r="BJ62" s="64"/>
+      <c r="BK62" s="64"/>
+      <c r="BL62" s="64"/>
+      <c r="BM62" s="47"/>
     </row>
-    <row r="63" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D63" s="5"/>
+    <row r="63" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="4"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -10924,7 +11039,7 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E61">
+  <conditionalFormatting sqref="E9:E62">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10938,7 +11053,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL61">
+  <conditionalFormatting sqref="I7:BL62">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
@@ -10958,7 +11073,7 @@
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BL60">
+  <conditionalFormatting sqref="I10:BL61">
     <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
@@ -10975,7 +11090,7 @@
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I61:BL61">
+  <conditionalFormatting sqref="I62:BL62">
     <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
@@ -10996,14 +11111,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{DFFD23FF-9FE8-42D1-8B69-600D9BF05AA3}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C60" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C61" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{40D643B7-C378-45A2-A932-672EA7F96D14}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A50:A60" xr:uid="{16EF2781-8358-4BE0-BED4-7AAF228778DA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A61" xr:uid="{59304489-FD95-4DFE-BAF7-57A94B8EB2FD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A51:A61" xr:uid="{16EF2781-8358-4BE0-BED4-7AAF228778DA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A62" xr:uid="{59304489-FD95-4DFE-BAF7-57A94B8EB2FD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Project information starting in cell B11 through cell G11. _x000a_Enter Milestone Description, select a Category, assign someone to the task, and enter the progress, start date, and number of days for the task to start charting._x000a_" sqref="A11" xr:uid="{4DD4ED10-9AD6-4E16-B98D-780C2836D133}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row contains headers for the project schedule.  B9 through G9 contains schedule information.  Cells I9 through BL9 contain the first letter of each day of the week for the date above that heading._x000a_All project timeline charting is auto generated." sqref="A9" xr:uid="{EF7E1D0C-1D4A-4ADD-A37B-656B82D2F645}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A scrollbar is in cells I8 through BL8. _x000a_To jump forward or backward in the timeline, enter a value of 0 or higher in cell C7._x000a_A value of 0 takes you to the beginning of the chart." sqref="A8" xr:uid="{9B040C77-1487-444F-9200-4040ACDB2DA8}"/>
@@ -11031,7 +11146,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>31750</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>57150</xdr:rowOff>
                   </from>
@@ -11039,7 +11154,7 @@
                     <xdr:col>64</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11068,7 +11183,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E61</xm:sqref>
+          <xm:sqref>E9:E62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{3EF75A3E-8286-4296-914E-C8F63A2E14FB}">
@@ -11087,7 +11202,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I61:BL61</xm:sqref>
+          <xm:sqref>I62:BL62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="32" id="{C84307BC-4E4D-4989-9D21-88D6AEB0AFD2}">
@@ -11106,7 +11221,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BL60</xm:sqref>
+          <xm:sqref>I10:BL61</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -11391,6 +11506,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -11407,15 +11531,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11440,6 +11555,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11449,12 +11572,4 @@
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>